<commit_message>
derniers retours et ajustements
</commit_message>
<xml_diff>
--- a/src/data/projets/data.xlsx
+++ b/src/data/projets/data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="172">
   <si>
     <t>code_projet</t>
   </si>
@@ -101,6 +101,9 @@
     <t>France</t>
   </si>
   <si>
+    <t>350 000</t>
+  </si>
+  <si>
     <t>DCE,  Livraison Janvier 2021</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
     <t>Orléans</t>
   </si>
   <si>
+    <t>200 000</t>
+  </si>
+  <si>
     <t>Chantier,  Livraison Janvier 2020</t>
   </si>
   <si>
@@ -170,6 +176,9 @@
     <t>92</t>
   </si>
   <si>
+    <t>110 000</t>
+  </si>
+  <si>
     <t>Livré, Janv 2019</t>
   </si>
   <si>
@@ -209,6 +218,9 @@
     <t>75</t>
   </si>
   <si>
+    <t>100 000</t>
+  </si>
+  <si>
     <t>Maud Saget Architecte</t>
   </si>
   <si>
@@ -239,6 +251,9 @@
     <t>RÉHABILITATION D'UN IMMEUBLE DE BUREAUX POUR LE GROUPE EALIS</t>
   </si>
   <si>
+    <t>1 800 000</t>
+  </si>
+  <si>
     <t>Livré, Juillet 2019</t>
   </si>
   <si>
@@ -278,6 +293,9 @@
     <t>56</t>
   </si>
   <si>
+    <t>3 500 000</t>
+  </si>
+  <si>
     <t>DCE, Livraison 2021</t>
   </si>
   <si>
@@ -315,6 +333,9 @@
   </si>
   <si>
     <t>49</t>
+  </si>
+  <si>
+    <t>150 000</t>
   </si>
   <si>
     <t>Livré, Avril 2018</t>
@@ -360,6 +381,9 @@
     <t>Chateauneuf-sur-Loiret</t>
   </si>
   <si>
+    <t>1 200 000</t>
+  </si>
+  <si>
     <t>Chantier,  Livraison Aout 2020</t>
   </si>
   <si>
@@ -393,6 +417,9 @@
     <t>Quelque part en Sologne</t>
   </si>
   <si>
+    <t>300 000</t>
+  </si>
+  <si>
     <t>Esquisse</t>
   </si>
   <si>
@@ -445,6 +472,9 @@
   </si>
   <si>
     <t>Hauts-de-Seine</t>
+  </si>
+  <si>
+    <t>180 000</t>
   </si>
   <si>
     <t>Livré, Dec 2017</t>
@@ -598,7 +628,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -615,9 +645,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1817,62 +1844,62 @@
       <c r="H2" s="5">
         <v>200</v>
       </c>
-      <c r="I2" s="6">
-        <v>350000</v>
+      <c r="I2" t="s" s="4">
+        <v>29</v>
       </c>
       <c r="J2" s="5">
         <v>12</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>42369</v>
       </c>
       <c r="L2" t="s" s="4">
-        <v>29</v>
-      </c>
-      <c r="M2" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="M2" s="7"/>
       <c r="N2" t="s" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="5">
         <v>190</v>
       </c>
       <c r="R2" t="s" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="5">
         <v>60</v>
       </c>
       <c r="T2" t="s" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U2" t="s" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V2" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W2" t="s" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="46.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s" s="4">
         <v>26</v>
@@ -1886,68 +1913,68 @@
       <c r="H3" s="5">
         <v>50</v>
       </c>
-      <c r="I3" s="6">
-        <v>200000</v>
+      <c r="I3" t="s" s="4">
+        <v>42</v>
       </c>
       <c r="J3" s="5">
         <v>11</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>42247</v>
       </c>
       <c r="L3" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="M3" s="8"/>
+        <v>43</v>
+      </c>
+      <c r="M3" s="7"/>
       <c r="N3" t="s" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O3" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="5">
         <v>115</v>
       </c>
       <c r="R3" t="s" s="4">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="S3" s="5">
         <v>30</v>
       </c>
       <c r="T3" t="s" s="4">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="U3" t="s" s="4">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V3" t="s" s="4">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="W3" t="s" s="4">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="35.65" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s" s="4">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s" s="4">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s" s="4">
         <v>28</v>
@@ -1955,68 +1982,68 @@
       <c r="H4" s="5">
         <v>90</v>
       </c>
-      <c r="I4" s="6">
-        <v>110000</v>
+      <c r="I4" t="s" s="4">
+        <v>54</v>
       </c>
       <c r="J4" s="5">
         <v>10</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>41943</v>
       </c>
       <c r="L4" t="s" s="4">
-        <v>52</v>
-      </c>
-      <c r="M4" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="M4" s="7"/>
       <c r="N4" t="s" s="4">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="O4" t="s" s="4">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="P4" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q4" s="5">
         <v>75</v>
       </c>
       <c r="R4" t="s" s="4">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="S4" s="5">
         <v>20</v>
       </c>
       <c r="T4" t="s" s="4">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="U4" t="s" s="4">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="V4" t="s" s="4">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="W4" t="s" s="4">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" ht="35.65" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s" s="4">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s" s="4">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s" s="4">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s" s="4">
         <v>28</v>
@@ -2024,64 +2051,64 @@
       <c r="H5" s="5">
         <v>150</v>
       </c>
-      <c r="I5" s="6">
-        <v>100000</v>
+      <c r="I5" t="s" s="4">
+        <v>68</v>
       </c>
       <c r="J5" s="5">
         <v>9</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>41973</v>
       </c>
       <c r="L5" t="s" s="4">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M5" t="s" s="4">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="N5" t="s" s="4">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="O5" t="s" s="4">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="P5" t="s" s="4">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="5">
         <v>110</v>
       </c>
       <c r="R5" t="s" s="4">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="S5" s="5">
         <v>30</v>
       </c>
       <c r="T5" t="s" s="4">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="U5" t="s" s="4">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="V5" t="s" s="4">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="W5" t="s" s="4">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" ht="57.65" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s" s="4">
         <v>26</v>
@@ -2095,68 +2122,68 @@
       <c r="H6" s="5">
         <v>650</v>
       </c>
-      <c r="I6" s="6">
-        <v>1800000</v>
+      <c r="I6" t="s" s="4">
+        <v>79</v>
       </c>
       <c r="J6" s="5">
         <v>8</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>41973</v>
       </c>
       <c r="L6" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="M6" s="8"/>
+        <v>80</v>
+      </c>
+      <c r="M6" s="7"/>
       <c r="N6" t="s" s="4">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="O6" t="s" s="4">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="P6" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="5">
         <v>175</v>
       </c>
       <c r="R6" t="s" s="4">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="S6" s="5">
         <v>60</v>
       </c>
       <c r="T6" t="s" s="4">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U6" t="s" s="4">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="V6" t="s" s="4">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="W6" t="s" s="4">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" ht="35.65" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s" s="4">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s" s="4">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s" s="4">
         <v>28</v>
@@ -2164,68 +2191,68 @@
       <c r="H7" s="5">
         <v>1020</v>
       </c>
-      <c r="I7" s="6">
-        <v>3500000</v>
+      <c r="I7" t="s" s="4">
+        <v>93</v>
       </c>
       <c r="J7" s="5">
         <v>7</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>42247</v>
       </c>
       <c r="L7" t="s" s="4">
-        <v>88</v>
-      </c>
-      <c r="M7" s="8"/>
+        <v>94</v>
+      </c>
+      <c r="M7" s="7"/>
       <c r="N7" t="s" s="4">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="O7" t="s" s="4">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="P7" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q7" s="5">
         <v>210</v>
       </c>
       <c r="R7" t="s" s="4">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="S7" s="5">
         <v>115</v>
       </c>
       <c r="T7" t="s" s="4">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="U7" t="s" s="4">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="V7" t="s" s="4">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="W7" t="s" s="4">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" ht="46.65" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s" s="4">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s" s="4">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s" s="4">
         <v>28</v>
@@ -2233,62 +2260,62 @@
       <c r="H8" s="5">
         <v>170</v>
       </c>
-      <c r="I8" s="6">
-        <v>150000</v>
+      <c r="I8" t="s" s="4">
+        <v>107</v>
       </c>
       <c r="J8" s="5">
         <v>6</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>41820</v>
       </c>
       <c r="L8" t="s" s="4">
-        <v>101</v>
-      </c>
-      <c r="M8" s="8"/>
+        <v>108</v>
+      </c>
+      <c r="M8" s="7"/>
       <c r="N8" t="s" s="4">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="O8" t="s" s="4">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="P8" t="s" s="4">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="Q8" s="5">
         <v>70</v>
       </c>
       <c r="R8" t="s" s="4">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="S8" s="5">
         <v>30</v>
       </c>
       <c r="T8" t="s" s="4">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="U8" t="s" s="4">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="V8" t="s" s="4">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="W8" t="s" s="4">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" ht="57.65" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s" s="4">
         <v>26</v>
@@ -2302,62 +2329,62 @@
       <c r="H9" s="5">
         <v>720</v>
       </c>
-      <c r="I9" s="6">
-        <v>1200000</v>
+      <c r="I9" t="s" s="4">
+        <v>120</v>
       </c>
       <c r="J9" s="5">
         <v>5</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>41973</v>
       </c>
       <c r="L9" t="s" s="4">
-        <v>113</v>
-      </c>
-      <c r="M9" s="8"/>
+        <v>121</v>
+      </c>
+      <c r="M9" s="7"/>
       <c r="N9" t="s" s="4">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="O9" t="s" s="4">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="P9" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="5">
         <v>140</v>
       </c>
       <c r="R9" t="s" s="4">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="S9" s="5">
         <v>115</v>
       </c>
       <c r="T9" t="s" s="4">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="U9" t="s" s="4">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="V9" t="s" s="4">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="W9" t="s" s="4">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" ht="35.65" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s" s="4">
         <v>26</v>
@@ -2371,60 +2398,60 @@
       <c r="H10" s="5">
         <v>110</v>
       </c>
-      <c r="I10" s="6">
-        <v>300000</v>
+      <c r="I10" t="s" s="4">
+        <v>132</v>
       </c>
       <c r="J10" s="5">
         <v>4</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="6"/>
       <c r="L10" t="s" s="4">
-        <v>124</v>
-      </c>
-      <c r="M10" s="8"/>
+        <v>133</v>
+      </c>
+      <c r="M10" s="7"/>
       <c r="N10" t="s" s="4">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="O10" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P10" t="s" s="4">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Q10" s="5">
         <v>55</v>
       </c>
       <c r="R10" t="s" s="4">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="S10" s="5">
         <v>40</v>
       </c>
       <c r="T10" t="s" s="4">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="U10" t="s" s="4">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="V10" t="s" s="4">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="W10" t="s" s="4">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" ht="35.65" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s" s="4">
         <v>26</v>
@@ -2438,66 +2465,66 @@
       <c r="H11" s="5">
         <v>320</v>
       </c>
-      <c r="I11" s="6">
-        <v>200000</v>
+      <c r="I11" t="s" s="4">
+        <v>42</v>
       </c>
       <c r="J11" s="5">
         <v>3</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>41729</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
       <c r="N11" t="s" s="4">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="O11" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P11" t="s" s="4">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="Q11" s="5">
         <v>60</v>
       </c>
       <c r="R11" t="s" s="4">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="S11" s="5">
         <v>45</v>
       </c>
       <c r="T11" t="s" s="4">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="U11" t="s" s="4">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="V11" t="s" s="4">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="W11" t="s" s="4">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" ht="46.65" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="E12" t="s" s="4">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="F12" t="s" s="4">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s" s="4">
         <v>28</v>
@@ -2505,111 +2532,111 @@
       <c r="H12" s="5">
         <v>110</v>
       </c>
-      <c r="I12" s="6">
-        <v>180000</v>
+      <c r="I12" t="s" s="4">
+        <v>151</v>
       </c>
       <c r="J12" s="5">
         <v>2</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>41274</v>
       </c>
       <c r="L12" t="s" s="4">
-        <v>142</v>
-      </c>
-      <c r="M12" s="8"/>
+        <v>152</v>
+      </c>
+      <c r="M12" s="7"/>
       <c r="N12" t="s" s="4">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="O12" t="s" s="4">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="P12" t="s" s="4">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Q12" s="5">
         <v>130</v>
       </c>
       <c r="R12" t="s" s="4">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="S12" s="5">
         <v>60</v>
       </c>
       <c r="T12" t="s" s="4">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="U12" t="s" s="4">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="V12" t="s" s="4">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="W12" t="s" s="4">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" ht="46.65" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s" s="4">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="F13" t="s" s="4">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="G13" t="s" s="4">
         <v>28</v>
       </c>
       <c r="H13" t="s" s="4">
-        <v>154</v>
-      </c>
-      <c r="I13" s="8"/>
+        <v>164</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="5">
         <v>1</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
       <c r="N13" t="s" s="4">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="O13" t="s" s="4">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="P13" t="s" s="4">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="Q13" s="5">
         <v>80</v>
       </c>
       <c r="R13" t="s" s="4">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="S13" s="5">
         <v>105</v>
       </c>
       <c r="T13" t="s" s="4">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="U13" t="s" s="4">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="V13" t="s" s="4">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="W13" t="s" s="4">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change red cedar to bois ...
</commit_message>
<xml_diff>
--- a/src/data/projets/data.xlsx
+++ b/src/data/projets/data.xlsx
@@ -536,16 +536,16 @@
     <t>Chantier,  Livraison Aout 2020</t>
   </si>
   <si>
-    <t>Red cedar</t>
+    <t>Bois thermo-chauffé</t>
   </si>
   <si>
     <t>Bureaux</t>
   </si>
   <si>
-    <t>EB12-redcedar-CAROTTE.jpg</t>
-  </si>
-  <si>
-    <t>EB12-REDCEDAR-BASEDEDONNEES.jpg</t>
+    <t>EB12-BOISTHERMOCHAUFFE-CAROTTE.jpg</t>
+  </si>
+  <si>
+    <t>EB12-BOISTHERMOCHAUFFE-BASEDEDONNEES.jpg</t>
   </si>
   <si>
     <t>BUREAUX-1</t>
@@ -1884,7 +1884,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="23" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="17" width="16.3516" style="1" customWidth="1"/>
+    <col min="18" max="18" width="66.4375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.3516" style="1" customWidth="1"/>
+    <col min="20" max="20" width="54.0703" style="1" customWidth="1"/>
+    <col min="21" max="23" width="16.3516" style="1" customWidth="1"/>
     <col min="24" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
first draft new db
</commit_message>
<xml_diff>
--- a/src/data/projets/data.xlsx
+++ b/src/data/projets/data.xlsx
@@ -3832,7 +3832,9 @@
       <c r="R22" t="s" s="4">
         <v>81</v>
       </c>
-      <c r="S22" s="7"/>
+      <c r="S22" s="5">
+        <v>240</v>
+      </c>
       <c r="T22" s="4"/>
       <c r="U22" s="5">
         <v>115</v>

</xml_diff>